<commit_message>
test case answer test update
test case answer test update
</commit_message>
<xml_diff>
--- a/Documents/FM_Test_case answer test.xlsx
+++ b/Documents/FM_Test_case answer test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>No</t>
   </si>
@@ -109,15 +109,6 @@
   </si>
   <si>
     <t>khi hoàn thành đề thi , thông tin câu trả lời được lưu trong database và xét kết quả của đề thi</t>
-  </si>
-  <si>
-    <t>check điểm của bài thi</t>
-  </si>
-  <si>
-    <t>xét số câu đúng và sai của đề thi và hiện số điểm của bài thi</t>
-  </si>
-  <si>
-    <t>sau khi hoàn thành đề thi , thí sinh có thể biết kết quả ngay khi bấm nút hoàn thành</t>
   </si>
 </sst>
 </file>
@@ -201,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -234,18 +225,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,29 +735,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>7</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18">
-        <v>3</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>9</v>
-      </c>
+    <row r="14" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
@@ -779,7 +757,7 @@
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="16"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
@@ -789,7 +767,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="B17" s="16"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="9"/>

</xml_diff>

<commit_message>
update test case answer test
update test case answer test
</commit_message>
<xml_diff>
--- a/Documents/FM_Test_case answer test.xlsx
+++ b/Documents/FM_Test_case answer test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>No</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>khi hoàn thành đề thi , thông tin câu trả lời được lưu trong database và xét kết quả của đề thi</t>
+  </si>
+  <si>
+    <t>check câu làm sai</t>
+  </si>
+  <si>
+    <t>chọn câu làm sai (màu đỏ) sẽ hiện câu đúng màu xanh lá cây</t>
+  </si>
+  <si>
+    <t>check đáp án câu bị sai và đổi màu đáp án đúng</t>
+  </si>
+  <si>
+    <t>check điểm bài thi</t>
+  </si>
+  <si>
+    <t>check số câu đúng và chấm điểm theo thang điểm 100</t>
+  </si>
+  <si>
+    <t>check số câu đúng của đề thi và tính điểm theo công thức :( 100/a)*b . Trong đó : a là số câu của đề thi , b là số câu đúng</t>
   </si>
 </sst>
 </file>
@@ -132,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -179,15 +197,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -223,21 +232,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,7 +551,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,29 +744,57 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+    <row r="14" spans="1:8" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17">
+        <v>3</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="19">
+        <v>3</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="17"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
@@ -767,7 +804,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="B17" s="17"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="9"/>

</xml_diff>